<commit_message>
updated from pagination to url to filter to 1000 items per category
</commit_message>
<xml_diff>
--- a/watsons_data_2.xlsx
+++ b/watsons_data_2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="481">
   <si>
     <t>id</t>
   </si>
@@ -478,6 +478,21 @@
     <t>https://api.watsons.com.my/medias/Oxy-Blackhead-Clearing-Wash-BP-65525.jpg?context=bWFzdGVyfGZyb250L2NhdHwzNTQ2fGltYWdlL2pwZWd8ZnJvbnQvY2F0L2hmZC9oMDQvODkwMzA2MDAyOTQ3MC5qcGd8OWY5ZTkxOGM4MGI2OTQ0ZDk0ZTdmZDA1ZmZjOGUxZDY4NGY0ZGMxNjFjZGE0YjAwNDAzNzMwYWM5ODA0NDA2Mw</t>
   </si>
   <si>
+    <t>BP_21603</t>
+  </si>
+  <si>
+    <t>OXY Acne &amp; Oil Control Foam Wash 150ml</t>
+  </si>
+  <si>
+    <t>https://www.watsons.com.my/acne-&amp;-oil-control-foam-wash-150ml/p/BP_21603</t>
+  </si>
+  <si>
+    <t>https://api.watsons.com.my/medias/Acne-Oil-Control-Foam-Wash-150ml-BP-21603.jpg?context=bWFzdGVyfGZyb250L2NhdHw5MzUyfGltYWdlL2pwZWd8ZnJvbnQvY2F0L2g1OS9oZjIvOTAxMTkxNTEyODg2Mi5qcGd8MGQyNmRlNmIwZDI5NmQ5ODZkYzMyNmY4M2MxZGY0ZWEwNjhhZjE2MjRhZmYwYTFjYzlmOGY5MDcyMWE0Mjg1NQ</t>
+  </si>
+  <si>
+    <t>Sold Out</t>
+  </si>
+  <si>
     <t>BP_18748</t>
   </si>
   <si>
@@ -1306,24 +1321,6 @@
     <t>58.65</t>
   </si>
   <si>
-    <t>BP_67090</t>
-  </si>
-  <si>
-    <t>HADA LABO Goku Jyun 3-in-1 Micellar Cleansing Water 380ml</t>
-  </si>
-  <si>
-    <t>https://www.watsons.com.my/goku-jyun-3-in-1-micellar-cleansing-water-380ml/p/BP_67090</t>
-  </si>
-  <si>
-    <t>https://api.watsons.com.my/medias/Goku-Jyun-3-in-1-Micellar-Cleansing-Water-380ml-BP-67090.jpg?context=bWFzdGVyfGZyb250L2NhdHw1ODg1fGltYWdlL2pwZWd8ZnJvbnQvY2F0LzkwMjUxNzIxNzY5MjYuanBnfGRiNTBlODM3ZmM3YmMwODE2NmEzYjMxODZmZTkyODdhMDU3NjhiOGU1NzQ1YzNkY2EzMGNhMzg5MzhlYmVjMzc</t>
-  </si>
-  <si>
-    <t>46.13</t>
-  </si>
-  <si>
-    <t>65.90</t>
-  </si>
-  <si>
     <t>BP_94489</t>
   </si>
   <si>
@@ -1390,6 +1387,51 @@
     <t>78.90</t>
   </si>
   <si>
+    <t>BP_28645</t>
+  </si>
+  <si>
+    <t>HADA LABO PLUS + Plus for Sensitive Skin Hydra Creamy Wash 100g</t>
+  </si>
+  <si>
+    <t>https://www.watsons.com.my/%2B-plus-for-sensitive-skin-hydra-creamy-wash-100g/p/BP_28645</t>
+  </si>
+  <si>
+    <t>https://api.watsons.com.my/medias/-Plus-for-Sensitive-Skin-Hydra-Creamy-Wash-100g-BP-28645.jpg?context=bWFzdGVyfGZyb250L2NhdHw1OTc2fGltYWdlL2pwZWd8ZnJvbnQvY2F0L2g1MS9oNGUvODk4OTAwODE5OTcxMC5qcGd8ZTdjN2M2NzgzOGRiYWM5YWNkY2ZjNTVkNzNhNmM2OGJhZDg0ZWMxNjJjNTlmNjBmOWMzMjMyMTExMzkyYWYwZg</t>
+  </si>
+  <si>
+    <t>29.90</t>
+  </si>
+  <si>
+    <t>BP_94478</t>
+  </si>
+  <si>
+    <t>HADA LABO PLUS + Brightening Facial Mask 1's</t>
+  </si>
+  <si>
+    <t>https://www.watsons.com.my/%2B-brightening-facial-mask-1's/p/BP_94478</t>
+  </si>
+  <si>
+    <t>https://api.watsons.com.my/medias/Brightening-Facial-Mask-1s-BP-94478.jpg?context=bWFzdGVyfGZyb250L2NhdHw2Mjk1fGltYWdlL2pwZWd8ZnJvbnQvY2F0LzkwMjkyNDYzNTM0MzguanBnfDlhYzUzY2NhOTFiZWEzOTMwOWYwYzllOWNiMGFlM2QzMDAxZjQ5NTJjZTY5YzQyODJhZjg3NWVjZjI2ZGZiNDE</t>
+  </si>
+  <si>
+    <t>BP_28649</t>
+  </si>
+  <si>
+    <t>HADA LABO PLUS + Plus for Sensitive Skin Hydra Milk 90ml</t>
+  </si>
+  <si>
+    <t>https://www.watsons.com.my/%2B-plus-for-sensitive-skin-hydra-milk-90ml/p/BP_28649</t>
+  </si>
+  <si>
+    <t>https://api.watsons.com.my/medias/cat-front-BP-28649.jpg?context=bWFzdGVyfGZyb250L2NhdHw1MjI4fGltYWdlL2pwZWd8ZnJvbnQvY2F0L2hhOS9oOWMvOTM2ODk4ODY0NzQ1NC5qcGd8ZGNlOTgwYjI4M2FiMDJhZjU3MmE3ODdmYmQ1Y2M2ODFiMzVmNGM3MGQ5N2I5OTBjNjExNGZjNTZlN2VmZjU1YQ</t>
+  </si>
+  <si>
+    <t>47.92</t>
+  </si>
+  <si>
+    <t>59.90</t>
+  </si>
+  <si>
     <t>BP_94476</t>
   </si>
   <si>
@@ -1412,51 +1454,6 @@
   </si>
   <si>
     <t>https://api.watsons.com.my/medias/Nourishing-Facial-Mask-1s-BP-94477.jpg?context=bWFzdGVyfGZyb250L2NhdHw2MjE3fGltYWdlL2pwZWd8ZnJvbnQvY2F0LzkwMjQxMTEyODAxNTguanBnfDE1NjBhOWNmOTlkM2I4NGUyNGMzYTU3YjNmZmZlZTI2N2Q3NjJmZjVhYjM1YWMyYTIzZDhkN2VjOWJhNGVmNjk</t>
-  </si>
-  <si>
-    <t>BP_94478</t>
-  </si>
-  <si>
-    <t>HADA LABO PLUS + Brightening Facial Mask 1's</t>
-  </si>
-  <si>
-    <t>https://www.watsons.com.my/%2B-brightening-facial-mask-1's/p/BP_94478</t>
-  </si>
-  <si>
-    <t>https://api.watsons.com.my/medias/Brightening-Facial-Mask-1s-BP-94478.jpg?context=bWFzdGVyfGZyb250L2NhdHw2Mjk1fGltYWdlL2pwZWd8ZnJvbnQvY2F0LzkwMjkyNDYzNTM0MzguanBnfDlhYzUzY2NhOTFiZWEzOTMwOWYwYzllOWNiMGFlM2QzMDAxZjQ5NTJjZTY5YzQyODJhZjg3NWVjZjI2ZGZiNDE</t>
-  </si>
-  <si>
-    <t>BP_28649</t>
-  </si>
-  <si>
-    <t>HADA LABO PLUS + Plus for Sensitive Skin Hydra Milk 90ml</t>
-  </si>
-  <si>
-    <t>https://www.watsons.com.my/%2B-plus-for-sensitive-skin-hydra-milk-90ml/p/BP_28649</t>
-  </si>
-  <si>
-    <t>https://api.watsons.com.my/medias/cat-front-BP-28649.jpg?context=bWFzdGVyfGZyb250L2NhdHw1MjI4fGltYWdlL2pwZWd8ZnJvbnQvY2F0L2hhOS9oOWMvOTM2ODk4ODY0NzQ1NC5qcGd8ZGNlOTgwYjI4M2FiMDJhZjU3MmE3ODdmYmQ1Y2M2ODFiMzVmNGM3MGQ5N2I5OTBjNjExNGZjNTZlN2VmZjU1YQ</t>
-  </si>
-  <si>
-    <t>47.92</t>
-  </si>
-  <si>
-    <t>59.90</t>
-  </si>
-  <si>
-    <t>BP_28645</t>
-  </si>
-  <si>
-    <t>HADA LABO PLUS + Plus for Sensitive Skin Hydra Creamy Wash 100g</t>
-  </si>
-  <si>
-    <t>https://www.watsons.com.my/%2B-plus-for-sensitive-skin-hydra-creamy-wash-100g/p/BP_28645</t>
-  </si>
-  <si>
-    <t>https://api.watsons.com.my/medias/-Plus-for-Sensitive-Skin-Hydra-Creamy-Wash-100g-BP-28645.jpg?context=bWFzdGVyfGZyb250L2NhdHw1OTc2fGltYWdlL2pwZWd8ZnJvbnQvY2F0L2g1MS9oNGUvODk4OTAwODE5OTcxMC5qcGd8ZTdjN2M2NzgzOGRiYWM5YWNkY2ZjNTVkNzNhNmM2OGJhZDg0ZWMxNjJjNTlmNjBmOWMzMjMyMTExMzkyYWYwZg</t>
-  </si>
-  <si>
-    <t>29.90</t>
   </si>
 </sst>
 </file>
@@ -2780,55 +2777,58 @@
       <c r="D30" t="s">
         <v>158</v>
       </c>
+      <c r="E30" t="s">
+        <v>159</v>
+      </c>
       <c r="F30" t="s">
         <v>15</v>
       </c>
       <c r="G30" t="s">
-        <v>159</v>
+        <v>16</v>
       </c>
       <c r="H30" t="s">
-        <v>160</v>
+        <v>17</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
       </c>
       <c r="J30">
-        <v>0.29999999999999993</v>
+        <v>0.5</v>
       </c>
       <c r="K30">
-        <v>7.949999999999999</v>
+        <v>12.45</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31" t="s">
         <v>161</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>162</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>163</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" t="s">
         <v>164</v>
-      </c>
-      <c r="F31" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" t="s">
-        <v>165</v>
       </c>
       <c r="H31" t="s">
         <v>165</v>
       </c>
       <c r="I31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>0.29999999999999993</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>7.949999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -2880,74 +2880,74 @@
         <v>15</v>
       </c>
       <c r="G33" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="H33" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="I33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>0.29999999999999993</v>
+        <v>0</v>
       </c>
       <c r="K33">
-        <v>7.949999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B34" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C34" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D34" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F34" t="s">
         <v>15</v>
       </c>
       <c r="G34" t="s">
-        <v>64</v>
+        <v>164</v>
       </c>
       <c r="H34" t="s">
-        <v>64</v>
+        <v>165</v>
       </c>
       <c r="I34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>0.29999999999999993</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>7.949999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B35" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C35" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D35" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F35" t="s">
         <v>15</v>
       </c>
       <c r="G35" t="s">
-        <v>183</v>
+        <v>64</v>
       </c>
       <c r="H35" t="s">
-        <v>183</v>
+        <v>64</v>
       </c>
       <c r="I35" t="b">
         <v>0</v>
@@ -3043,135 +3043,135 @@
         <v>198</v>
       </c>
       <c r="H38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38">
-        <v>0.1499493414387031</v>
+        <v>0</v>
       </c>
       <c r="K38">
-        <v>14.799999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>199</v>
+      </c>
+      <c r="B39" t="s">
         <v>200</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>201</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>202</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" t="s">
         <v>203</v>
       </c>
-      <c r="F39" t="s">
-        <v>15</v>
-      </c>
-      <c r="G39" t="s">
-        <v>183</v>
-      </c>
       <c r="H39" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="I39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39">
-        <v>0</v>
+        <v>0.1499493414387031</v>
       </c>
       <c r="K39">
-        <v>0</v>
+        <v>14.799999999999997</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B40" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C40" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D40" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F40" t="s">
         <v>15</v>
       </c>
       <c r="G40" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="H40" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="I40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>0.29999999999999993</v>
+        <v>0</v>
       </c>
       <c r="K40">
-        <v>7.949999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B41" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C41" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D41" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F41" t="s">
         <v>15</v>
       </c>
       <c r="G41" t="s">
-        <v>212</v>
+        <v>164</v>
       </c>
       <c r="H41" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
       <c r="I41" t="b">
         <v>1</v>
       </c>
       <c r="J41">
-        <v>0.19999999999999996</v>
+        <v>0.29999999999999993</v>
       </c>
       <c r="K41">
-        <v>22</v>
+        <v>7.949999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>213</v>
+      </c>
+      <c r="B42" t="s">
         <v>214</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>215</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>216</v>
       </c>
-      <c r="D42" t="s">
+      <c r="F42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" t="s">
         <v>217</v>
       </c>
-      <c r="F42" t="s">
-        <v>15</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>218</v>
-      </c>
-      <c r="H42" t="s">
-        <v>219</v>
       </c>
       <c r="I42" t="b">
         <v>1</v>
@@ -3180,39 +3180,39 @@
         <v>0.19999999999999996</v>
       </c>
       <c r="K42">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>219</v>
+      </c>
+      <c r="B43" t="s">
         <v>220</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>221</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>222</v>
       </c>
-      <c r="D43" t="s">
+      <c r="F43" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" t="s">
         <v>223</v>
-      </c>
-      <c r="F43" t="s">
-        <v>15</v>
-      </c>
-      <c r="G43" t="s">
-        <v>224</v>
       </c>
       <c r="H43" t="s">
         <v>224</v>
       </c>
       <c r="I43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43">
-        <v>0</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="K43">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -3267,71 +3267,71 @@
         <v>234</v>
       </c>
       <c r="H45" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45">
-        <v>0.29999999999999993</v>
+        <v>0</v>
       </c>
       <c r="K45">
-        <v>14.969999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>235</v>
+      </c>
+      <c r="B46" t="s">
         <v>236</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>237</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>238</v>
       </c>
-      <c r="D46" t="s">
+      <c r="F46" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" t="s">
         <v>239</v>
       </c>
-      <c r="F46" t="s">
-        <v>15</v>
-      </c>
-      <c r="G46" t="s">
-        <v>188</v>
-      </c>
       <c r="H46" t="s">
-        <v>188</v>
+        <v>240</v>
       </c>
       <c r="I46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>0.29999999999999993</v>
       </c>
       <c r="K46">
-        <v>0</v>
+        <v>14.969999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B47" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C47" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D47" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F47" t="s">
         <v>15</v>
       </c>
       <c r="G47" t="s">
-        <v>244</v>
+        <v>193</v>
       </c>
       <c r="H47" t="s">
-        <v>244</v>
+        <v>193</v>
       </c>
       <c r="I47" t="b">
         <v>0</v>
@@ -3360,10 +3360,10 @@
         <v>15</v>
       </c>
       <c r="G48" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="H48" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
@@ -3377,153 +3377,153 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>250</v>
+      </c>
+      <c r="B49" t="s">
+        <v>251</v>
+      </c>
+      <c r="C49" t="s">
+        <v>252</v>
+      </c>
+      <c r="D49" t="s">
+        <v>253</v>
+      </c>
+      <c r="F49" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" t="s">
         <v>249</v>
       </c>
-      <c r="B49" t="s">
-        <v>250</v>
-      </c>
-      <c r="C49" t="s">
-        <v>251</v>
-      </c>
-      <c r="D49" t="s">
-        <v>252</v>
-      </c>
-      <c r="F49" t="s">
-        <v>15</v>
-      </c>
-      <c r="G49" t="s">
-        <v>234</v>
-      </c>
       <c r="H49" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="I49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49">
-        <v>0.29999999999999993</v>
+        <v>0</v>
       </c>
       <c r="K49">
-        <v>14.969999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B50" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C50" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D50" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F50" t="s">
         <v>15</v>
       </c>
       <c r="G50" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="H50" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="I50" t="b">
         <v>1</v>
       </c>
       <c r="J50">
-        <v>0.14991789819376022</v>
+        <v>0.29999999999999993</v>
       </c>
       <c r="K50">
-        <v>9.129999999999995</v>
+        <v>14.969999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>258</v>
+      </c>
+      <c r="B51" t="s">
         <v>259</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>260</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>261</v>
       </c>
-      <c r="D51" t="s">
+      <c r="F51" t="s">
+        <v>15</v>
+      </c>
+      <c r="G51" t="s">
         <v>262</v>
       </c>
-      <c r="F51" t="s">
-        <v>15</v>
-      </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>263</v>
       </c>
-      <c r="H51" t="s">
-        <v>264</v>
-      </c>
       <c r="I51" t="b">
         <v>1</v>
       </c>
       <c r="J51">
-        <v>0.15000000000000002</v>
+        <v>0.14991789819376022</v>
       </c>
       <c r="K51">
-        <v>7.950000000000003</v>
+        <v>9.129999999999995</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>264</v>
+      </c>
+      <c r="B52" t="s">
         <v>265</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>266</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>267</v>
       </c>
-      <c r="D52" t="s">
+      <c r="F52" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" t="s">
         <v>268</v>
       </c>
-      <c r="F52" t="s">
-        <v>15</v>
-      </c>
-      <c r="G52" t="s">
-        <v>170</v>
-      </c>
       <c r="H52" t="s">
-        <v>170</v>
+        <v>269</v>
       </c>
       <c r="I52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52">
-        <v>0</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="K52">
-        <v>0</v>
+        <v>7.950000000000003</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B53" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C53" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D53" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F53" t="s">
         <v>15</v>
       </c>
       <c r="G53" t="s">
-        <v>273</v>
+        <v>175</v>
       </c>
       <c r="H53" t="s">
-        <v>273</v>
+        <v>175</v>
       </c>
       <c r="I53" t="b">
         <v>0</v>
@@ -3552,51 +3552,51 @@
         <v>15</v>
       </c>
       <c r="G54" t="s">
-        <v>159</v>
+        <v>278</v>
       </c>
       <c r="H54" t="s">
-        <v>160</v>
+        <v>278</v>
       </c>
       <c r="I54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J54">
-        <v>0.29999999999999993</v>
+        <v>0</v>
       </c>
       <c r="K54">
-        <v>7.949999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B55" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C55" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D55" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F55" t="s">
         <v>15</v>
       </c>
       <c r="G55" t="s">
-        <v>282</v>
+        <v>164</v>
       </c>
       <c r="H55" t="s">
-        <v>282</v>
+        <v>165</v>
       </c>
       <c r="I55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55">
-        <v>0</v>
+        <v>0.29999999999999993</v>
       </c>
       <c r="K55">
-        <v>0</v>
+        <v>7.949999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -3648,10 +3648,10 @@
         <v>15</v>
       </c>
       <c r="G57" t="s">
-        <v>244</v>
+        <v>292</v>
       </c>
       <c r="H57" t="s">
-        <v>244</v>
+        <v>292</v>
       </c>
       <c r="I57" t="b">
         <v>0</v>
@@ -3665,25 +3665,25 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B58" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C58" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D58" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
       </c>
       <c r="G58" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="H58" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="I58" t="b">
         <v>0</v>
@@ -3697,25 +3697,25 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B59" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C59" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D59" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F59" t="s">
         <v>15</v>
       </c>
       <c r="G59" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="H59" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="I59" t="b">
         <v>0</v>
@@ -3747,167 +3747,167 @@
         <v>305</v>
       </c>
       <c r="H60" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I60" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J60">
-        <v>0.19999999999999996</v>
+        <v>0</v>
       </c>
       <c r="K60">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>306</v>
+      </c>
+      <c r="B61" t="s">
         <v>307</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>308</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>309</v>
       </c>
-      <c r="D61" t="s">
+      <c r="F61" t="s">
+        <v>15</v>
+      </c>
+      <c r="G61" t="s">
         <v>310</v>
       </c>
-      <c r="F61" t="s">
-        <v>15</v>
-      </c>
-      <c r="G61" t="s">
-        <v>193</v>
-      </c>
       <c r="H61" t="s">
-        <v>193</v>
+        <v>311</v>
       </c>
       <c r="I61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61">
-        <v>0</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="K61">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B62" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C62" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D62" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F62" t="s">
         <v>15</v>
       </c>
       <c r="G62" t="s">
-        <v>315</v>
+        <v>198</v>
       </c>
       <c r="H62" t="s">
-        <v>316</v>
+        <v>198</v>
       </c>
       <c r="I62" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J62">
-        <v>0.20000000000000007</v>
+        <v>0</v>
       </c>
       <c r="K62">
-        <v>15.180000000000007</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>316</v>
+      </c>
+      <c r="B63" t="s">
         <v>317</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>318</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>319</v>
       </c>
-      <c r="D63" t="s">
+      <c r="F63" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63" t="s">
         <v>320</v>
       </c>
-      <c r="F63" t="s">
-        <v>15</v>
-      </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>321</v>
       </c>
-      <c r="H63" t="s">
-        <v>322</v>
-      </c>
       <c r="I63" t="b">
         <v>1</v>
       </c>
       <c r="J63">
-        <v>0.15000000000000002</v>
+        <v>0.20000000000000007</v>
       </c>
       <c r="K63">
-        <v>9.899999999999999</v>
+        <v>15.180000000000007</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>322</v>
+      </c>
+      <c r="B64" t="s">
         <v>323</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>324</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>325</v>
       </c>
-      <c r="D64" t="s">
+      <c r="F64" t="s">
+        <v>15</v>
+      </c>
+      <c r="G64" t="s">
         <v>326</v>
       </c>
-      <c r="F64" t="s">
-        <v>15</v>
-      </c>
-      <c r="G64" t="s">
-        <v>322</v>
-      </c>
       <c r="H64" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="I64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J64">
-        <v>0</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="K64">
-        <v>0</v>
+        <v>9.899999999999999</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>328</v>
+      </c>
+      <c r="B65" t="s">
+        <v>329</v>
+      </c>
+      <c r="C65" t="s">
+        <v>330</v>
+      </c>
+      <c r="D65" t="s">
+        <v>331</v>
+      </c>
+      <c r="F65" t="s">
+        <v>15</v>
+      </c>
+      <c r="G65" t="s">
         <v>327</v>
       </c>
-      <c r="B65" t="s">
-        <v>328</v>
-      </c>
-      <c r="C65" t="s">
-        <v>329</v>
-      </c>
-      <c r="D65" t="s">
-        <v>330</v>
-      </c>
-      <c r="F65" t="s">
-        <v>15</v>
-      </c>
-      <c r="G65" t="s">
-        <v>64</v>
-      </c>
       <c r="H65" t="s">
-        <v>64</v>
+        <v>327</v>
       </c>
       <c r="I65" t="b">
         <v>0</v>
@@ -3921,25 +3921,25 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B66" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C66" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D66" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F66" t="s">
         <v>15</v>
       </c>
       <c r="G66" t="s">
-        <v>244</v>
+        <v>64</v>
       </c>
       <c r="H66" t="s">
-        <v>244</v>
+        <v>64</v>
       </c>
       <c r="I66" t="b">
         <v>0</v>
@@ -3953,34 +3953,34 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B67" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C67" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D67" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="F67" t="s">
         <v>15</v>
       </c>
       <c r="G67" t="s">
-        <v>339</v>
+        <v>249</v>
       </c>
       <c r="H67" t="s">
-        <v>199</v>
+        <v>249</v>
       </c>
       <c r="I67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J67">
-        <v>0.20000000000000007</v>
+        <v>0</v>
       </c>
       <c r="K67">
-        <v>19.74000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -4000,42 +4000,42 @@
         <v>15</v>
       </c>
       <c r="G68" t="s">
-        <v>321</v>
+        <v>344</v>
       </c>
       <c r="H68" t="s">
-        <v>322</v>
+        <v>204</v>
       </c>
       <c r="I68" t="b">
         <v>1</v>
       </c>
       <c r="J68">
-        <v>0.15000000000000002</v>
+        <v>0.20000000000000007</v>
       </c>
       <c r="K68">
-        <v>9.899999999999999</v>
+        <v>19.74000000000001</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B69" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C69" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D69" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="F69" t="s">
         <v>15</v>
       </c>
       <c r="G69" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="H69" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="I69" t="b">
         <v>1</v>
@@ -4049,34 +4049,34 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B70" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C70" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D70" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="F70" t="s">
         <v>15</v>
       </c>
       <c r="G70" t="s">
-        <v>352</v>
+        <v>326</v>
       </c>
       <c r="H70" t="s">
-        <v>352</v>
+        <v>327</v>
       </c>
       <c r="I70" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J70">
-        <v>0</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="K70">
-        <v>0</v>
+        <v>9.899999999999999</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -4096,10 +4096,10 @@
         <v>15</v>
       </c>
       <c r="G71" t="s">
-        <v>188</v>
+        <v>357</v>
       </c>
       <c r="H71" t="s">
-        <v>188</v>
+        <v>357</v>
       </c>
       <c r="I71" t="b">
         <v>0</v>
@@ -4113,80 +4113,80 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B72" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C72" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D72" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="F72" t="s">
         <v>15</v>
       </c>
       <c r="G72" t="s">
-        <v>361</v>
+        <v>193</v>
       </c>
       <c r="H72" t="s">
-        <v>362</v>
+        <v>193</v>
       </c>
       <c r="I72" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J72">
-        <v>0.20000000000000007</v>
+        <v>0</v>
       </c>
       <c r="K72">
-        <v>18.700000000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>362</v>
+      </c>
+      <c r="B73" t="s">
         <v>363</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>364</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>365</v>
       </c>
-      <c r="D73" t="s">
+      <c r="F73" t="s">
+        <v>15</v>
+      </c>
+      <c r="G73" t="s">
         <v>366</v>
       </c>
-      <c r="F73" t="s">
-        <v>15</v>
-      </c>
-      <c r="G73" t="s">
-        <v>193</v>
-      </c>
       <c r="H73" t="s">
-        <v>193</v>
+        <v>367</v>
       </c>
       <c r="I73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J73">
-        <v>0</v>
+        <v>0.20000000000000007</v>
       </c>
       <c r="K73">
-        <v>0</v>
+        <v>18.700000000000003</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B74" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C74" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D74" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="F74" t="s">
         <v>15</v>
@@ -4195,71 +4195,71 @@
         <v>198</v>
       </c>
       <c r="H74" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J74">
-        <v>0.1499493414387031</v>
+        <v>0</v>
       </c>
       <c r="K74">
-        <v>14.799999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B75" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C75" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D75" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F75" t="s">
         <v>15</v>
       </c>
       <c r="G75" t="s">
-        <v>287</v>
+        <v>203</v>
       </c>
       <c r="H75" t="s">
-        <v>287</v>
+        <v>204</v>
       </c>
       <c r="I75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J75">
-        <v>0</v>
+        <v>0.1499493414387031</v>
       </c>
       <c r="K75">
-        <v>0</v>
+        <v>14.799999999999997</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B76" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C76" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D76" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F76" t="s">
         <v>15</v>
       </c>
       <c r="G76" t="s">
-        <v>170</v>
+        <v>292</v>
       </c>
       <c r="H76" t="s">
-        <v>170</v>
+        <v>292</v>
       </c>
       <c r="I76" t="b">
         <v>0</v>
@@ -4273,25 +4273,25 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B77" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C77" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D77" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="F77" t="s">
         <v>15</v>
       </c>
       <c r="G77" t="s">
-        <v>383</v>
+        <v>175</v>
       </c>
       <c r="H77" t="s">
-        <v>383</v>
+        <v>175</v>
       </c>
       <c r="I77" t="b">
         <v>0</v>
@@ -4384,10 +4384,10 @@
         <v>15</v>
       </c>
       <c r="G80" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="H80" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="I80" t="b">
         <v>0</v>
@@ -4401,25 +4401,25 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>399</v>
+      </c>
+      <c r="B81" t="s">
+        <v>400</v>
+      </c>
+      <c r="C81" t="s">
+        <v>401</v>
+      </c>
+      <c r="D81" t="s">
+        <v>402</v>
+      </c>
+      <c r="F81" t="s">
+        <v>15</v>
+      </c>
+      <c r="G81" t="s">
         <v>398</v>
       </c>
-      <c r="B81" t="s">
-        <v>399</v>
-      </c>
-      <c r="C81" t="s">
-        <v>400</v>
-      </c>
-      <c r="D81" t="s">
-        <v>401</v>
-      </c>
-      <c r="F81" t="s">
-        <v>15</v>
-      </c>
-      <c r="G81" t="s">
-        <v>402</v>
-      </c>
       <c r="H81" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="I81" t="b">
         <v>0</v>
@@ -4448,10 +4448,10 @@
         <v>15</v>
       </c>
       <c r="G82" t="s">
-        <v>282</v>
+        <v>407</v>
       </c>
       <c r="H82" t="s">
-        <v>282</v>
+        <v>407</v>
       </c>
       <c r="I82" t="b">
         <v>0</v>
@@ -4465,25 +4465,25 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B83" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C83" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D83" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="F83" t="s">
         <v>15</v>
       </c>
       <c r="G83" t="s">
-        <v>411</v>
+        <v>287</v>
       </c>
       <c r="H83" t="s">
-        <v>411</v>
+        <v>287</v>
       </c>
       <c r="I83" t="b">
         <v>0</v>
@@ -4512,19 +4512,19 @@
         <v>15</v>
       </c>
       <c r="G84" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="H84" t="s">
         <v>416</v>
       </c>
       <c r="I84" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J84">
-        <v>0.30000000000000004</v>
+        <v>0</v>
       </c>
       <c r="K84">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -4544,19 +4544,19 @@
         <v>15</v>
       </c>
       <c r="G85" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="H85" t="s">
         <v>421</v>
       </c>
       <c r="I85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J85">
-        <v>0</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K85">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -4576,10 +4576,10 @@
         <v>15</v>
       </c>
       <c r="G86" t="s">
-        <v>64</v>
+        <v>426</v>
       </c>
       <c r="H86" t="s">
-        <v>64</v>
+        <v>426</v>
       </c>
       <c r="I86" t="b">
         <v>0</v>
@@ -4593,34 +4593,34 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B87" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C87" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D87" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="F87" t="s">
         <v>15</v>
       </c>
       <c r="G87" t="s">
-        <v>430</v>
+        <v>64</v>
       </c>
       <c r="H87" t="s">
-        <v>393</v>
+        <v>64</v>
       </c>
       <c r="I87" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J87">
-        <v>0.15000000000000002</v>
+        <v>0</v>
       </c>
       <c r="K87">
-        <v>10.350000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -4643,39 +4643,39 @@
         <v>435</v>
       </c>
       <c r="H88" t="s">
-        <v>436</v>
+        <v>398</v>
       </c>
       <c r="I88" t="b">
         <v>1</v>
       </c>
       <c r="J88">
-        <v>0.30000000000000004</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="K88">
-        <v>19.770000000000003</v>
+        <v>10.350000000000001</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>436</v>
+      </c>
+      <c r="B89" t="s">
         <v>437</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>438</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
         <v>439</v>
       </c>
-      <c r="D89" t="s">
+      <c r="F89" t="s">
+        <v>15</v>
+      </c>
+      <c r="G89" t="s">
         <v>440</v>
       </c>
-      <c r="F89" t="s">
-        <v>15</v>
-      </c>
-      <c r="G89" t="s">
+      <c r="H89" t="s">
         <v>441</v>
-      </c>
-      <c r="H89" t="s">
-        <v>442</v>
       </c>
       <c r="I89" t="b">
         <v>1</v>
@@ -4689,25 +4689,25 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>442</v>
+      </c>
+      <c r="B90" t="s">
         <v>443</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>444</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>445</v>
       </c>
-      <c r="D90" t="s">
-        <v>446</v>
-      </c>
       <c r="F90" t="s">
         <v>15</v>
       </c>
       <c r="G90" t="s">
+        <v>440</v>
+      </c>
+      <c r="H90" t="s">
         <v>441</v>
-      </c>
-      <c r="H90" t="s">
-        <v>442</v>
       </c>
       <c r="I90" t="b">
         <v>1</v>
@@ -4721,25 +4721,25 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>446</v>
+      </c>
+      <c r="B91" t="s">
         <v>447</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>448</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>449</v>
       </c>
-      <c r="D91" t="s">
+      <c r="F91" t="s">
+        <v>15</v>
+      </c>
+      <c r="G91" t="s">
         <v>450</v>
       </c>
-      <c r="F91" t="s">
-        <v>15</v>
-      </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>451</v>
-      </c>
-      <c r="H91" t="s">
-        <v>452</v>
       </c>
       <c r="I91" t="b">
         <v>1</v>
@@ -4753,25 +4753,25 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>452</v>
+      </c>
+      <c r="B92" t="s">
         <v>453</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>454</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>455</v>
       </c>
-      <c r="D92" t="s">
+      <c r="F92" t="s">
+        <v>15</v>
+      </c>
+      <c r="G92" t="s">
         <v>456</v>
       </c>
-      <c r="F92" t="s">
-        <v>15</v>
-      </c>
-      <c r="G92" t="s">
+      <c r="H92" t="s">
         <v>457</v>
-      </c>
-      <c r="H92" t="s">
-        <v>458</v>
       </c>
       <c r="I92" t="b">
         <v>1</v>
@@ -4785,34 +4785,34 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>458</v>
+      </c>
+      <c r="B93" t="s">
         <v>459</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>460</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>461</v>
       </c>
-      <c r="D93" t="s">
+      <c r="F93" t="s">
+        <v>15</v>
+      </c>
+      <c r="G93" t="s">
         <v>462</v>
       </c>
-      <c r="F93" t="s">
-        <v>15</v>
-      </c>
-      <c r="G93" t="s">
-        <v>441</v>
-      </c>
       <c r="H93" t="s">
-        <v>442</v>
+        <v>462</v>
       </c>
       <c r="I93" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J93">
-        <v>0.30000000000000004</v>
+        <v>0</v>
       </c>
       <c r="K93">
-        <v>2.9700000000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -4832,10 +4832,10 @@
         <v>15</v>
       </c>
       <c r="G94" t="s">
+        <v>440</v>
+      </c>
+      <c r="H94" t="s">
         <v>441</v>
-      </c>
-      <c r="H94" t="s">
-        <v>442</v>
       </c>
       <c r="I94" t="b">
         <v>1</v>
@@ -4864,51 +4864,51 @@
         <v>15</v>
       </c>
       <c r="G95" t="s">
-        <v>441</v>
+        <v>471</v>
       </c>
       <c r="H95" t="s">
-        <v>442</v>
+        <v>472</v>
       </c>
       <c r="I95" t="b">
         <v>1</v>
       </c>
       <c r="J95">
-        <v>0.30000000000000004</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="K95">
-        <v>2.9700000000000006</v>
+        <v>11.979999999999997</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B96" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C96" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D96" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="F96" t="s">
         <v>15</v>
       </c>
       <c r="G96" t="s">
-        <v>475</v>
+        <v>440</v>
       </c>
       <c r="H96" t="s">
-        <v>476</v>
+        <v>441</v>
       </c>
       <c r="I96" t="b">
         <v>1</v>
       </c>
       <c r="J96">
-        <v>0.19999999999999996</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K96">
-        <v>11.979999999999997</v>
+        <v>2.9700000000000006</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -4928,19 +4928,19 @@
         <v>15</v>
       </c>
       <c r="G97" t="s">
-        <v>481</v>
+        <v>440</v>
       </c>
       <c r="H97" t="s">
-        <v>481</v>
+        <v>441</v>
       </c>
       <c r="I97" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J97">
-        <v>0</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K97">
-        <v>0</v>
+        <v>2.9700000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>